<commit_message>
update ws/app + infra qrm009
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qrm009.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qrm009.xlsx
@@ -16,8 +16,6 @@
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ケア対象者一覧!#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">ケア対象者一覧!#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -80,115 +78,96 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>&amp;=$retirePayItemT1001</t>
+  </si>
+  <si>
+    <t>&amp;=$retirePayItemT2001</t>
+  </si>
+  <si>
+    <t>&amp;=$retirePayItemT2002</t>
+  </si>
+  <si>
+    <t>&amp;=$retirePayItemT2003</t>
+  </si>
+  <si>
+    <t>&amp;=$retirePayItemT2004</t>
+  </si>
+  <si>
+    <t>&amp;=$retirePayItemT2005</t>
+  </si>
+  <si>
+    <t>&amp;=$retirePayItemT2006</t>
+  </si>
+  <si>
+    <t>&amp;=$retirePayItemT2007</t>
+  </si>
+  <si>
+    <t>&amp;=$retirePayItemT3001</t>
+  </si>
+  <si>
+    <t>&amp;=data.personalBasicDto.retireReason</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.trialPeriodSet</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.exclusionYears</t>
+  </si>
+  <si>
+    <t>&amp;=data.personalBasicDto.workingYears</t>
+  </si>
+  <si>
+    <t>&amp;=data.personalBasicDto.otherOfficerWorkingYears</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.totalPaymentMoney</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.incomeTaxMoney</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.cityTaxMoney</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.prefectureTaxMoney</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.deductionMoney1</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.deductionMoney2</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.deductionMoney3</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.totalDeductionMoney</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.actualRecieveMoney</t>
+  </si>
+  <si>
+    <t>&amp;=data.retirementPaymentDto.statementMemo</t>
+  </si>
+  <si>
+    <t>&amp;=data.companyMasterDto.companyName</t>
+  </si>
+  <si>
     <t>&amp;=data.personalBasicDto.personName</t>
+  </si>
+  <si>
+    <t>&amp;=data.personalBasicDto.joinDate</t>
+  </si>
+  <si>
+    <t>&amp;=data.personalBasicDto.retireDate</t>
+  </si>
+  <si>
+    <t>&amp;=$currentDate(bean)</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>&amp;=data.personalBasicDto.joinDate</t>
+    <t>&amp;=$companyAddress</t>
     <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.personalBasicDto.retireDate</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.personalBasicDto.retireReason</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.trialPeriodSet</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.exclusionYears</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.personalBasicDto.workingYears</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.personalBasicDto.otherOfficerWorkingYears</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.incomeTaxMoney</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.cityTaxMoney</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.prefectureTaxMoney</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.deductionMoney1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.deductionMoney2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.deductionMoney3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.totalDeductionMoney</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.actualRecieveMoney</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.statementMemo</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.companyMasterDto.companyName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.companyMasterDto.address1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=$currentDate</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=data.retirementPaymentDto.totalPaymentMoney</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT1001</t>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT2001</t>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT2002</t>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT2003</t>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT2004</t>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT2005</t>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT2006</t>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT2007</t>
-  </si>
-  <si>
-    <t>&amp;=$retirePayItemT3001</t>
   </si>
 </sst>
 </file>
@@ -199,7 +178,7 @@
     <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="177" formatCode="#,##0;[Red]#,##0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,7 +392,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -454,88 +433,91 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -864,10 +846,10 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:N28"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="26.75" style="1" customWidth="1"/>
@@ -882,29 +864,29 @@
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="53.25" customHeight="1">
-      <c r="D1" s="40" t="s">
+    <row r="1" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="M1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N1" s="14"/>
-    </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="M1" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="41"/>
+    </row>
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="12"/>
       <c r="E2" s="15" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -914,17 +896,17 @@
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
-      <c r="N2" s="17"/>
-    </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="N2" s="39"/>
+    </row>
+    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="3"/>
       <c r="E3" s="15" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -934,63 +916,62 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="N3" s="39"/>
+    </row>
+    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="3"/>
       <c r="E4" s="15" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="G4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="15"/>
       <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="17"/>
-    </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="15"/>
       <c r="G5" s="15" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="I5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="15"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="3"/>
       <c r="E6" s="15" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -1000,17 +981,17 @@
       <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
-      <c r="N6" s="17"/>
-    </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1">
-      <c r="A7" s="39" t="s">
+      <c r="N6" s="39"/>
+    </row>
+    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="3"/>
       <c r="E7" s="15" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -1020,33 +1001,33 @@
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
-      <c r="N7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:14" ht="18" customHeight="1">
-      <c r="A9" s="37"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="36" t="s">
+      <c r="N7" s="39"/>
+    </row>
+    <row r="8" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="5"/>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1">
-      <c r="A10" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
+    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="8"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1055,39 +1036,39 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="35"/>
+      <c r="L10" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="34"/>
       <c r="N10" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25" customHeight="1"/>
-    <row r="12" spans="1:14" ht="18" customHeight="1">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="36" t="s">
+    <row r="11" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1">
-      <c r="A13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1096,20 +1077,20 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="24"/>
+      <c r="L13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="23"/>
       <c r="N13" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1">
-      <c r="A14" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1118,20 +1099,20 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" s="35"/>
+      <c r="L14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="34"/>
       <c r="N14" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1">
-      <c r="A15" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1140,20 +1121,20 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="35"/>
+      <c r="L15" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="34"/>
       <c r="N15" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1">
-      <c r="A16" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -1162,20 +1143,20 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="M16" s="35"/>
+      <c r="L16" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="34"/>
       <c r="N16" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="18" customHeight="1">
-      <c r="A17" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1184,20 +1165,20 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17" s="35"/>
+      <c r="L17" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="34"/>
       <c r="N17" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1">
-      <c r="A18" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1206,20 +1187,20 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="M18" s="35"/>
+      <c r="L18" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" s="34"/>
       <c r="N18" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1">
-      <c r="A19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
+    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1228,21 +1209,21 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" s="35"/>
+      <c r="L19" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" s="34"/>
       <c r="N19" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="13.5" customHeight="1"/>
-    <row r="21" spans="1:14" ht="18" customHeight="1">
-      <c r="A21" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
+    <row r="20" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1251,18 +1232,18 @@
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="M21" s="23"/>
-      <c r="N21" s="21" t="s">
+      <c r="L21" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="M21" s="22"/>
+      <c r="N21" s="20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="18" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
+    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1271,53 +1252,53 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="22"/>
-    </row>
-    <row r="23" spans="1:14" ht="12.75" customHeight="1"/>
-    <row r="24" spans="1:14" ht="18" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="21"/>
+    </row>
+    <row r="23" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="21"/>
-    </row>
-    <row r="25" spans="1:14" ht="18" customHeight="1">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="22"/>
-    </row>
-    <row r="27" spans="1:14" ht="18" customHeight="1">
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="20"/>
+    </row>
+    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="27"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="21"/>
+    </row>
+    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -1331,12 +1312,12 @@
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
     </row>
-    <row r="28" spans="1:14" ht="18" customHeight="1">
+    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -1351,7 +1332,17 @@
       <c r="N28" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="43">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="E7:N7"/>
     <mergeCell ref="D9:J9"/>
@@ -1364,30 +1355,14 @@
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L19:M19"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="D12:J12"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="L14:M14"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="D24:N25"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
     <mergeCell ref="C27:N27"/>
     <mergeCell ref="C28:N28"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A17:C17"/>
@@ -1396,9 +1371,14 @@
     <mergeCell ref="N21:N22"/>
     <mergeCell ref="L21:M22"/>
     <mergeCell ref="A21:C22"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="D24:N25"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <pageMargins left="0.47244094488188998" right="0.85312500000000002" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageMargins left="0.47244094488188998" right="0.47244094488188998" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="90" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>